<commit_message>
Fix duplicate ID detection and some invalid data in the good dataset
</commit_message>
<xml_diff>
--- a/packages/lan/__tests__/importers/test_definitions.xlsx
+++ b/packages/lan/__tests__/importers/test_definitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="310">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -788,37 +788,22 @@
     <t xml:space="preserve">procedure-35081</t>
   </si>
   <si>
-    <t xml:space="preserve">Direct repair of aneurysm, pseudoaneurysm, or excision (partial or total) and graft insertion, with or without patch graft; for aneurysm, pseudoaneurysm, and associated occlusive disease, abdominal aorta</t>
+    <t xml:space="preserve">Direct repair of aneurysm, pseudoaneurysm, or excision (partial or total) and graft insertion, with or without patch graft</t>
   </si>
   <si>
     <t xml:space="preserve">procedure-35082</t>
   </si>
   <si>
-    <t xml:space="preserve">Direct repair of aneurysm, pseudoaneurysm, or excision (partial or total) and graft insertion, with or without patch graft; for ruptured aneurysm, abdominal aorta</t>
-  </si>
-  <si>
     <t xml:space="preserve">procedure-35091</t>
   </si>
   <si>
-    <t xml:space="preserve">Direct repair of aneurysm, pseudoaneurysm, or excision (partial or total) and graft insertion, with or without patch graft; for aneurysm, pseudoaneurysm, and associated occlusive disease, abdominal aorta involving visceral vessels (mesenteric, celiac, renal)</t>
-  </si>
-  <si>
     <t xml:space="preserve">procedure-35092</t>
   </si>
   <si>
-    <t xml:space="preserve">Direct repair of aneurysm, pseudoaneurysm, or excision (partial or total) and graft insertion, with or without patch graft; for ruptured aneurysm, abdominal aorta involving visceral vessels (mesenteric, celiac, renal)</t>
-  </si>
-  <si>
     <t xml:space="preserve">procedure-35102</t>
   </si>
   <si>
-    <t xml:space="preserve">Direct repair of aneurysm, pseudoaneurysm, or excision (partial or total) and graft insertion, with or without patch graft; for aneurysm, pseudoaneurysm, and associated occlusive disease, abdominal aorta involving iliac vessels (common, hypogastric, external)</t>
-  </si>
-  <si>
     <t xml:space="preserve">procedure-35103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direct repair of aneurysm, pseudoaneurysm, or excision (partial or total) and graft insertion, with or without patch graft; for ruptured aneurysm, abdominal aorta involving iliac vessels (common, hypogastric, external)</t>
   </si>
   <si>
     <t xml:space="preserve">procedure-23900</t>
@@ -1134,10 +1119,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B7" activeCellId="1" sqref="C6 B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
@@ -1245,13 +1230,13 @@
   </sheetPr>
   <dimension ref="A1:C1012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="168.41"/>
   </cols>
@@ -1319,62 +1304,62 @@
         <v>35082</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>35091</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>35092</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>35102</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>35103</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>23900</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5406,10 +5391,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="D15" activeCellId="1" sqref="C6 D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
@@ -5421,130 +5406,130 @@
         <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="G3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G8" s="7"/>
     </row>
@@ -5556,172 +5541,172 @@
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="G10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>295</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="2" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="2" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="2" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5852,10 +5837,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="C6 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.14"/>
   </cols>
@@ -8969,13 +8954,13 @@
   </sheetPr>
   <dimension ref="A1:C958"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B18" activeCellId="1" sqref="C6 B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="105.14"/>
@@ -11979,10 +11964,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="C6 A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12141,10 +12126,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="1" sqref="C6 A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12294,10 +12279,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C12" activeCellId="1" sqref="C6 C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12441,10 +12426,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="1" sqref="C6 B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.71"/>
   </cols>
@@ -16610,10 +16595,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="C29" activeCellId="1" sqref="C6 C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.86"/>
   </cols>
@@ -16895,10 +16880,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="1" sqref="C6 A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Refactor importers with a bit more separation of concerns
</commit_message>
<xml_diff>
--- a/packages/lan/__tests__/importers/test_definitions.xlsx
+++ b/packages/lan/__tests__/importers/test_definitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId2"/>
@@ -1119,10 +1119,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="1" sqref="C6 B7"/>
+      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
@@ -1230,13 +1230,13 @@
   </sheetPr>
   <dimension ref="A1:C1012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="168.41"/>
   </cols>
@@ -5391,10 +5391,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D15" activeCellId="1" sqref="C6 D15"/>
+      <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
@@ -5834,13 +5834,13 @@
   </sheetPr>
   <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="C6 A3"/>
+      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.14"/>
   </cols>
@@ -8957,10 +8957,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B18" activeCellId="1" sqref="C6 B18"/>
+      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="105.14"/>
@@ -11964,10 +11964,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="1" sqref="C6 A12"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12126,10 +12126,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="1" sqref="C6 A14"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12279,10 +12279,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C12" activeCellId="1" sqref="C6 C12"/>
+      <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -12426,10 +12426,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="1" sqref="C6 B17"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.71"/>
   </cols>
@@ -16595,10 +16595,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C29" activeCellId="1" sqref="C6 C29"/>
+      <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.86"/>
   </cols>
@@ -16880,10 +16880,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="1" sqref="C6 A5"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Switch to yup for validation
</commit_message>
<xml_diff>
--- a/packages/lan/__tests__/importers/test_definitions.xlsx
+++ b/packages/lan/__tests__/importers/test_definitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="418">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -597,10 +597,25 @@
     <t xml:space="preserve">invalid id</t>
   </si>
   <si>
+    <t xml:space="preserve">Invalid-id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Drug invalid id</t>
   </si>
   <si>
+    <t xml:space="preserve">Duplicate-code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Drug duplicate id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid-code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug invalid code</t>
   </si>
   <si>
     <t xml:space="preserve">allergy-penicillin</t>
@@ -1386,7 +1401,7 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
@@ -1806,35 +1821,35 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -1879,112 +1894,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>34830</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>34831</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>34832</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>35081</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>35082</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>35091</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>35092</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>35102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>35103</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>23900</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -2023,282 +2038,282 @@
         <v>123</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>124</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>373</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -2811,12 +2826,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2958,16 +2973,33 @@
       <c r="A14" s="0" t="s">
         <v>187</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>188</v>
+      </c>
       <c r="C14" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>182</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>190</v>
+      </c>
       <c r="C15" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -3009,112 +3041,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3156,112 +3188,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3303,112 +3335,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3453,112 +3485,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3603,112 +3635,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Find and link foreign keys while importing
</commit_message>
<xml_diff>
--- a/packages/lan/__tests__/importers/test_definitions.xlsx
+++ b/packages/lan/__tests__/importers/test_definitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="421">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -213,9 +213,6 @@
     <t xml:space="preserve">dateOfBirth</t>
   </si>
   <si>
-    <t xml:space="preserve">age</t>
-  </si>
-  <si>
     <t xml:space="preserve">sex</t>
   </si>
   <si>
@@ -243,7 +240,7 @@
     <t xml:space="preserve">male</t>
   </si>
   <si>
-    <t xml:space="preserve">B+</t>
+    <t xml:space="preserve">Alafua</t>
   </si>
   <si>
     <t xml:space="preserve">3aa63a3c-bb1e-4f3c-a185-ad18b5218256</t>
@@ -267,9 +264,6 @@
     <t xml:space="preserve">female</t>
   </si>
   <si>
-    <t xml:space="preserve">AB+</t>
-  </si>
-  <si>
     <t xml:space="preserve">f4d11593-9519-4229-abc7-378b62f36208</t>
   </si>
   <si>
@@ -288,9 +282,6 @@
     <t xml:space="preserve">Manuel</t>
   </si>
   <si>
-    <t xml:space="preserve">A+</t>
-  </si>
-  <si>
     <t xml:space="preserve">b612e53b-f0df-44f2-9adf-0efbce2b2d9f</t>
   </si>
   <si>
@@ -309,9 +300,6 @@
     <t xml:space="preserve">Dora</t>
   </si>
   <si>
-    <t xml:space="preserve">O+</t>
-  </si>
-  <si>
     <t xml:space="preserve">e324ef09-c525-4469-9ffb-21c21fd2ad27</t>
   </si>
   <si>
@@ -360,6 +348,9 @@
     <t xml:space="preserve">Scheffer</t>
   </si>
   <si>
+    <t xml:space="preserve">village-alamagoto</t>
+  </si>
+  <si>
     <t xml:space="preserve">53969c48-3b07-4851-8913-cb76f935f6ba</t>
   </si>
   <si>
@@ -378,6 +369,9 @@
     <t xml:space="preserve">Vincent</t>
   </si>
   <si>
+    <t xml:space="preserve">village-aleipata</t>
+  </si>
+  <si>
     <t xml:space="preserve">3de41550-9c10-4b9c-9468-0e1c76059e43</t>
   </si>
   <si>
@@ -390,6 +384,9 @@
     <t xml:space="preserve">Fusco</t>
   </si>
   <si>
+    <t xml:space="preserve">village-aleisa</t>
+  </si>
+  <si>
     <t xml:space="preserve">44da8ebb-c0ac-4eb8-b30f-24da73f30d4b</t>
   </si>
   <si>
@@ -402,6 +399,33 @@
     <t xml:space="preserve">Naicker</t>
   </si>
   <si>
+    <t xml:space="preserve">village-amaile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad-village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC123123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unfindable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">village-nowhere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid-village-fk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC123444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isnt</t>
+  </si>
+  <si>
     <t xml:space="preserve">code</t>
   </si>
   <si>
@@ -459,37 +483,22 @@
     <t xml:space="preserve">ALAFUA</t>
   </si>
   <si>
-    <t xml:space="preserve">Alafua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">village-alamagoto</t>
-  </si>
-  <si>
     <t xml:space="preserve">ALAMAGOTO</t>
   </si>
   <si>
     <t xml:space="preserve">Alamagoto</t>
   </si>
   <si>
-    <t xml:space="preserve">village-aleipata</t>
-  </si>
-  <si>
     <t xml:space="preserve">ALEIPATA</t>
   </si>
   <si>
     <t xml:space="preserve">Aleipata</t>
   </si>
   <si>
-    <t xml:space="preserve">village-aleisa</t>
-  </si>
-  <si>
     <t xml:space="preserve">ALEISA</t>
   </si>
   <si>
     <t xml:space="preserve">Aleisa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">village-amaile</t>
   </si>
   <si>
     <t xml:space="preserve">AMAILE</t>
@@ -1404,7 +1413,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1813,43 +1822,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -1886,120 +1895,120 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>34830</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>34831</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>34832</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>35081</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>35082</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>35091</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>35092</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>35102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>35103</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>23900</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2023,7 +2032,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2035,285 +2044,285 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -2332,12 +2341,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2345,6 +2354,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,290 +2385,342 @@
       <c r="I1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>68</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>23770.973599537</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="G3" s="4" t="n">
         <v>39304.8800810185</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>84</v>
       </c>
       <c r="G4" s="4" t="n">
         <v>38701.1676157407</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="G5" s="4" t="n">
         <v>38366.5308912037</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="G6" s="4" t="n">
         <v>24926.1681828704</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="G7" s="4" t="n">
         <v>31606.1075</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>108</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G8" s="4" t="n">
         <v>21608.5840740741</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>114</v>
       </c>
       <c r="G9" s="4" t="n">
         <v>21365.9580787037</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="E10" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>118</v>
-      </c>
       <c r="F10" s="0" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G10" s="4" t="n">
         <v>18750.24625</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>122</v>
       </c>
       <c r="G11" s="4" t="n">
         <v>34234.4166666667</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>77</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>34234.4166666667</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>34234.4166666667</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2681,7 +2743,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2694,120 +2756,120 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2828,7 +2890,7 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
@@ -2845,161 +2907,161 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3033,120 +3095,120 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3180,120 +3242,120 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3327,120 +3389,120 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3477,120 +3539,120 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -3627,120 +3689,120 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
595: Use correct field for lab test category import (#1034)
</commit_message>
<xml_diff>
--- a/packages/lan/__tests__/importers/test_definitions.xlsx
+++ b/packages/lan/__tests__/importers/test_definitions.xlsx
@@ -1189,7 +1189,7 @@
     <t xml:space="preserve">Malaria microscopy</t>
   </si>
   <si>
-    <t xml:space="preserve">category</t>
+    <t xml:space="preserve">labTestCategory</t>
   </si>
   <si>
     <t xml:space="preserve">resultType</t>
@@ -1333,7 +1333,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1439,7 +1439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1451,11 +1451,12 @@
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,7 +1839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1850,9 +1851,11 @@
       <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="168.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1988,7 +1991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2000,9 +2003,10 @@
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,7 +2076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2084,10 +2088,12 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,7 +2279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2282,17 +2288,20 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="46.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="46.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13109,7 +13118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13121,12 +13130,14 @@
       <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13506,7 +13517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13518,9 +13529,10 @@
       <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13656,7 +13668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13668,10 +13680,12 @@
       <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="105.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13848,7 +13862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13860,7 +13874,10 @@
       <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.5"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -13995,7 +14012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14007,7 +14024,10 @@
       <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.5"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -14142,7 +14162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14154,7 +14174,10 @@
       <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.5"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -14289,7 +14312,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14301,9 +14324,11 @@
       <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14439,7 +14464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14451,9 +14476,11 @@
       <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update test definitions to include facility links
</commit_message>
<xml_diff>
--- a/packages/lan/__tests__/importers/test_definitions.xlsx
+++ b/packages/lan/__tests__/importers/test_definitions.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="458">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -719,13 +719,13 @@
     <t xml:space="preserve">Carbamazepine</t>
   </si>
   <si>
-    <t xml:space="preserve">d7686384-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-Balwyn</t>
   </si>
   <si>
     <t xml:space="preserve">Balwyn</t>
   </si>
   <si>
-    <t xml:space="preserve">d7686686-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-HawthornEast</t>
   </si>
   <si>
     <t xml:space="preserve">HawthornEast</t>
@@ -734,13 +734,13 @@
     <t xml:space="preserve">Hawthorn East</t>
   </si>
   <si>
-    <t xml:space="preserve">d768678a-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-Kerang</t>
   </si>
   <si>
     <t xml:space="preserve">Kerang</t>
   </si>
   <si>
-    <t xml:space="preserve">d7686852-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-LakeCharm</t>
   </si>
   <si>
     <t xml:space="preserve">LakeCharm</t>
@@ -749,13 +749,13 @@
     <t xml:space="preserve">Lake Charm</t>
   </si>
   <si>
-    <t xml:space="preserve">d768691a-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-Marla</t>
   </si>
   <si>
     <t xml:space="preserve">Marla</t>
   </si>
   <si>
-    <t xml:space="preserve">d7686ac8-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-MontAlbert</t>
   </si>
   <si>
     <t xml:space="preserve">MontAlbert</t>
@@ -764,7 +764,7 @@
     <t xml:space="preserve">Mont Albert</t>
   </si>
   <si>
-    <t xml:space="preserve">d7686b90-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-NationalMedical</t>
   </si>
   <si>
     <t xml:space="preserve">NationalMedical</t>
@@ -773,7 +773,7 @@
     <t xml:space="preserve">National Medical</t>
   </si>
   <si>
-    <t xml:space="preserve">d7686c44-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-PortDouglas</t>
   </si>
   <si>
     <t xml:space="preserve">PortDouglas</t>
@@ -782,7 +782,7 @@
     <t xml:space="preserve">Port Douglas</t>
   </si>
   <si>
-    <t xml:space="preserve">d7686d02-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-SwanHill</t>
   </si>
   <si>
     <t xml:space="preserve">SwanHill</t>
@@ -791,13 +791,16 @@
     <t xml:space="preserve">Swan Hill</t>
   </si>
   <si>
-    <t xml:space="preserve">d7686e88-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facility-Thornbury</t>
   </si>
   <si>
     <t xml:space="preserve">Thornbury</t>
   </si>
   <si>
-    <t xml:space="preserve">c7378562-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">facilityId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">department-medical</t>
   </si>
   <si>
     <t xml:space="preserve">medical</t>
@@ -806,7 +809,7 @@
     <t xml:space="preserve">Medical</t>
   </si>
   <si>
-    <t xml:space="preserve">c73787ba-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-renal</t>
   </si>
   <si>
     <t xml:space="preserve">renal</t>
@@ -815,7 +818,7 @@
     <t xml:space="preserve">Renal</t>
   </si>
   <si>
-    <t xml:space="preserve">c73788aa-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-emergency</t>
   </si>
   <si>
     <t xml:space="preserve">emergency</t>
@@ -824,7 +827,7 @@
     <t xml:space="preserve">Emergency</t>
   </si>
   <si>
-    <t xml:space="preserve">c7378972-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-surgical</t>
   </si>
   <si>
     <t xml:space="preserve">surgical</t>
@@ -833,7 +836,7 @@
     <t xml:space="preserve">Surgical</t>
   </si>
   <si>
-    <t xml:space="preserve">c7378a3a-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-diabetes</t>
   </si>
   <si>
     <t xml:space="preserve">diabetes</t>
@@ -842,7 +845,7 @@
     <t xml:space="preserve">Diabetes</t>
   </si>
   <si>
-    <t xml:space="preserve">c7378c92-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-tuberculosis</t>
   </si>
   <si>
     <t xml:space="preserve">tuberculosis</t>
@@ -851,7 +854,7 @@
     <t xml:space="preserve">Tuberculosis</t>
   </si>
   <si>
-    <t xml:space="preserve">c7378d46-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-paediatric</t>
   </si>
   <si>
     <t xml:space="preserve">paediatric</t>
@@ -860,7 +863,7 @@
     <t xml:space="preserve">Paediatric</t>
   </si>
   <si>
-    <t xml:space="preserve">c7378e04-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-neonatal</t>
   </si>
   <si>
     <t xml:space="preserve">neonatal</t>
@@ -869,7 +872,7 @@
     <t xml:space="preserve">Neonatal</t>
   </si>
   <si>
-    <t xml:space="preserve">c7378eb8-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-antenatal</t>
   </si>
   <si>
     <t xml:space="preserve">antenatal</t>
@@ -878,7 +881,7 @@
     <t xml:space="preserve">Antenatal</t>
   </si>
   <si>
-    <t xml:space="preserve">c7378f76-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">department-laboratory</t>
   </si>
   <si>
     <t xml:space="preserve">laboratory</t>
@@ -887,7 +890,7 @@
     <t xml:space="preserve">Laboratory</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c2c02-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-bed1</t>
   </si>
   <si>
     <t xml:space="preserve">bed1</t>
@@ -896,7 +899,7 @@
     <t xml:space="preserve">Bed 1</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c2e6e-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-bed2</t>
   </si>
   <si>
     <t xml:space="preserve">bed2</t>
@@ -905,7 +908,7 @@
     <t xml:space="preserve">Bed 2</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c2f54-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-bed3</t>
   </si>
   <si>
     <t xml:space="preserve">bed3</t>
@@ -914,13 +917,13 @@
     <t xml:space="preserve">Bed 3</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c301c-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-diabetes</t>
   </si>
   <si>
     <t xml:space="preserve">Diabetes Clinic</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c30da-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-resus</t>
   </si>
   <si>
     <t xml:space="preserve">resus</t>
@@ -929,7 +932,7 @@
     <t xml:space="preserve">Resuscitation</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c3198-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-shortstay</t>
   </si>
   <si>
     <t xml:space="preserve">shortstay</t>
@@ -938,7 +941,7 @@
     <t xml:space="preserve">Short-Stay</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c3422-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-acute</t>
   </si>
   <si>
     <t xml:space="preserve">acute</t>
@@ -947,7 +950,7 @@
     <t xml:space="preserve">Acute Area</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c34e0-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-waiting</t>
   </si>
   <si>
     <t xml:space="preserve">waiting</t>
@@ -956,7 +959,7 @@
     <t xml:space="preserve">Waiting Area</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c35a8-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-location9</t>
   </si>
   <si>
     <t xml:space="preserve">location9</t>
@@ -965,7 +968,7 @@
     <t xml:space="preserve">Location 9</t>
   </si>
   <si>
-    <t xml:space="preserve">d31c365c-c8db-11eb-b8bc-0242ac130003</t>
+    <t xml:space="preserve">location-location10</t>
   </si>
   <si>
     <t xml:space="preserve">location10</t>
@@ -1412,7 +1415,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1518,7 +1521,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1530,12 +1533,11 @@
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,7 +1920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1930,11 +1932,9 @@
       <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,112 +1950,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -2070,7 +2070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2082,11 +2082,9 @@
       <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="168.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2102,112 +2100,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>34830</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>34831</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>34832</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>35081</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>35082</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>35091</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>35092</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>35102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>35103</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>23900</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -2222,7 +2220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2234,10 +2232,9 @@
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,46 +2250,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -2307,7 +2304,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2319,12 +2316,10 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,57 +2335,57 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,7 +2505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2522,17 +2517,14 @@
       <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="46.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2546,199 +2538,199 @@
         <v>132</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="I2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="I4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="I5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="I6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -2747,19 +2739,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -2768,42 +2760,42 @@
     </row>
     <row r="10" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -13349,7 +13341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13361,14 +13353,12 @@
       <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13748,7 +13738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13760,10 +13750,9 @@
       <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13899,7 +13888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -13911,12 +13900,10 @@
       <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="105.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14093,7 +14080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14105,10 +14092,7 @@
       <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.5"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -14243,20 +14227,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14271,7 +14256,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="0" t="s">
         <v>228</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -14282,7 +14267,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="0" t="s">
         <v>230</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -14293,7 +14278,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="0" t="s">
         <v>233</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -14304,7 +14289,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="0" t="s">
         <v>235</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -14315,7 +14300,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="0" t="s">
         <v>238</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -14326,7 +14311,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="0" t="s">
         <v>240</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -14337,7 +14322,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="0" t="s">
         <v>243</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -14348,7 +14333,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="0" t="s">
         <v>246</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -14359,7 +14344,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="0" t="s">
         <v>249</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -14370,7 +14355,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="0" t="s">
         <v>252</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -14395,22 +14380,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14423,115 +14407,148 @@
       <c r="C1" s="0" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>257</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>260</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>263</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>266</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>269</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>272</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>278</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>281</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -14546,21 +14563,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14573,115 +14590,148 @@
       <c r="C1" s="0" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>287</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>290</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>293</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>295</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>298</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>301</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>304</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>307</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>310</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -14696,7 +14746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14708,11 +14758,9 @@
       <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14728,112 +14776,112 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make Administered Vaccines importer idempotent
</commit_message>
<xml_diff>
--- a/packages/lan/__tests__/importers/test_definitions.xlsx
+++ b/packages/lan/__tests__/importers/test_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkennedy/proj/tamanu/packages/lan/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642AF382-280F-E24D-A4C9-400BF93434C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746F2257-010C-7245-B117-AFB7D4D8858A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="489">
   <si>
     <t>id</t>
   </si>
@@ -1495,6 +1495,18 @@
   </si>
   <si>
     <t>c4e16a1f-ce8c-4e92-b554-aa5a8d6441d8</t>
+  </si>
+  <si>
+    <t>administeredVaccineId</t>
+  </si>
+  <si>
+    <t>f41e29a3-609c-4d24-9e31-077551c05293</t>
+  </si>
+  <si>
+    <t>625ecfeb-557a-46d9-9195-8c49cde139d3</t>
+  </si>
+  <si>
+    <t>encounterId</t>
   </si>
 </sst>
 </file>
@@ -13641,122 +13653,132 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F135F617-0BF7-ED4D-9AB0-266A47D2EC17}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
-    <col min="9" max="9" width="34" customWidth="1"/>
-    <col min="10" max="10" width="26.5" customWidth="1"/>
-    <col min="11" max="11" width="33.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" customWidth="1"/>
+    <col min="10" max="10" width="34" customWidth="1"/>
+    <col min="11" max="11" width="26.5" customWidth="1"/>
+    <col min="12" max="12" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>488</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>459</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>463</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B2" t="s">
         <v>465</v>
       </c>
-      <c r="B2" s="6">
+      <c r="C2" s="6">
         <v>37665</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>466</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>464</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>482</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>480</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="B3" s="6">
+      <c r="C3" s="6">
         <v>37665</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>464</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>482</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>480</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>